<commit_message>
Added queues and resettable counter
</commit_message>
<xml_diff>
--- a/PBT/evaluation.xlsx
+++ b/PBT/evaluation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/Documents/IITM/certified-mrdts/PBT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66CBB90D-09FD-E642-8E90-24F7DD76469C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A00486CD-2264-4E40-8EAD-358BD67756D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="7" xr2:uid="{EBA8590F-3435-3740-9A14-214F762E4F04}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="1" activeTab="9" xr2:uid="{EBA8590F-3435-3740-9A14-214F762E4F04}"/>
   </bookViews>
   <sheets>
     <sheet name="ewflag_divergent_wo_fork" sheetId="1" r:id="rId1"/>
@@ -20,8 +20,10 @@
     <sheet name="lwwreg_wo_fork" sheetId="5" r:id="rId5"/>
     <sheet name="orset_divergent_wo_fork " sheetId="6" r:id="rId6"/>
     <sheet name="orset_wo_fork" sheetId="7" r:id="rId7"/>
-    <sheet name="orset_eff_wo_fork)" sheetId="9" r:id="rId8"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId9"/>
+    <sheet name="orset_eff_wo_fork" sheetId="9" r:id="rId8"/>
+    <sheet name="resettable_ctr_wo_fork" sheetId="10" r:id="rId9"/>
+    <sheet name="queue_wo_fork" sheetId="11" r:id="rId10"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId11"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -44,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="5">
   <si>
     <t>Time taken (s)</t>
   </si>
@@ -65,7 +67,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -91,6 +93,12 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -112,7 +120,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -120,6 +128,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2777,7 +2791,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'orset_eff_wo_fork)'!$B$1</c:f>
+              <c:f>orset_eff_wo_fork!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2819,7 +2833,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'orset_eff_wo_fork)'!$A$2:$A$8</c:f>
+              <c:f>orset_eff_wo_fork!$A$2:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2849,7 +2863,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'orset_eff_wo_fork)'!$C$2:$C$8</c:f>
+              <c:f>orset_eff_wo_fork!$C$2:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -3228,7 +3242,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'orset_eff_wo_fork)'!$B$1</c:f>
+              <c:f>orset_eff_wo_fork!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3270,7 +3284,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'orset_eff_wo_fork)'!$A$2:$A$8</c:f>
+              <c:f>orset_eff_wo_fork!$A$2:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -3300,7 +3314,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'orset_eff_wo_fork)'!$B$2:$B$8</c:f>
+              <c:f>orset_eff_wo_fork!$B$2:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -3627,6 +3641,1314 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>resettable_ctr_wo_fork!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Time taken (s)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:alpha val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw dist="25400" dir="2700000" algn="tl" rotWithShape="0">
+                <a:schemeClr val="accent1"/>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="22225">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>resettable_ctr_wo_fork!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>resettable_ctr_wo_fork!$C$2:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>264</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6784</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>246560</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11852544</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5E4F-8A4B-AAF1-2A0E1B45A25C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1942278720"/>
+        <c:axId val="1942007936"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1942278720"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:alpha val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                  <a:lnSpc>
+                    <a:spcPct val="100000"/>
+                  </a:lnSpc>
+                  <a:spcBef>
+                    <a:spcPts val="0"/>
+                  </a:spcBef>
+                  <a:spcAft>
+                    <a:spcPts val="0"/>
+                  </a:spcAft>
+                  <a:buClrTx/>
+                  <a:buSzTx/>
+                  <a:buFontTx/>
+                  <a:buNone/>
+                  <a:tabLst/>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="window" lastClr="FFFFFF"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="window" lastClr="FFFFFF"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t> |steps|</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                <a:lnSpc>
+                  <a:spcPct val="100000"/>
+                </a:lnSpc>
+                <a:spcBef>
+                  <a:spcPts val="0"/>
+                </a:spcBef>
+                <a:spcAft>
+                  <a:spcPts val="0"/>
+                </a:spcAft>
+                <a:buClrTx/>
+                <a:buSzTx/>
+                <a:buFontTx/>
+                <a:buNone/>
+                <a:tabLst/>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="window" lastClr="FFFFFF"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1942007936"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1942007936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:alpha val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                  <a:lnSpc>
+                    <a:spcPct val="100000"/>
+                  </a:lnSpc>
+                  <a:spcBef>
+                    <a:spcPts val="0"/>
+                  </a:spcBef>
+                  <a:spcAft>
+                    <a:spcPts val="0"/>
+                  </a:spcAft>
+                  <a:buClrTx/>
+                  <a:buSzTx/>
+                  <a:buFontTx/>
+                  <a:buNone/>
+                  <a:tabLst/>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="window" lastClr="FFFFFF"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="window" lastClr="FFFFFF"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>|configs|</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                <a:lnSpc>
+                  <a:spcPct val="100000"/>
+                </a:lnSpc>
+                <a:spcBef>
+                  <a:spcPts val="0"/>
+                </a:spcBef>
+                <a:spcAft>
+                  <a:spcPts val="0"/>
+                </a:spcAft>
+                <a:buClrTx/>
+                <a:buSzTx/>
+                <a:buFontTx/>
+                <a:buNone/>
+                <a:tabLst/>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="window" lastClr="FFFFFF"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1942278720"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="accent1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="accent1"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>resettable_ctr_wo_fork!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Time taken (s)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:alpha val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw dist="25400" dir="2700000" algn="tl" rotWithShape="0">
+                <a:schemeClr val="accent1"/>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="22225">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>resettable_ctr_wo_fork!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>resettable_ctr_wo_fork!$B$2:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5000000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.8999999999999998E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0449999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.4667000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.5190999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>141.505155</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1B65-9D42-9477-21F8DDD38B79}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1974682752"/>
+        <c:axId val="1975510720"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1974682752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:alpha val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                  <a:lnSpc>
+                    <a:spcPct val="100000"/>
+                  </a:lnSpc>
+                  <a:spcBef>
+                    <a:spcPts val="0"/>
+                  </a:spcBef>
+                  <a:spcAft>
+                    <a:spcPts val="0"/>
+                  </a:spcAft>
+                  <a:buClrTx/>
+                  <a:buSzTx/>
+                  <a:buFontTx/>
+                  <a:buNone/>
+                  <a:tabLst/>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="window" lastClr="FFFFFF"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="window" lastClr="FFFFFF"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t> |steps|</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                <a:lnSpc>
+                  <a:spcPct val="100000"/>
+                </a:lnSpc>
+                <a:spcBef>
+                  <a:spcPts val="0"/>
+                </a:spcBef>
+                <a:spcAft>
+                  <a:spcPts val="0"/>
+                </a:spcAft>
+                <a:buClrTx/>
+                <a:buSzTx/>
+                <a:buFontTx/>
+                <a:buNone/>
+                <a:tabLst/>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="window" lastClr="FFFFFF"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:alpha val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1975510720"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1975510720"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:alpha val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Time taken (s) </a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1974682752"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="accent1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="accent1"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>queue_wo_fork!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Time taken (s)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:alpha val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw dist="25400" dir="2700000" algn="tl" rotWithShape="0">
+                <a:schemeClr val="accent1"/>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="22225">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>queue_wo_fork!$A$2:$A$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>queue_wo_fork!$C$2:$C$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>264</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F1CB-F349-9694-619EF5D211C8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1942278720"/>
+        <c:axId val="1942007936"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1942278720"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:alpha val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                  <a:lnSpc>
+                    <a:spcPct val="100000"/>
+                  </a:lnSpc>
+                  <a:spcBef>
+                    <a:spcPts val="0"/>
+                  </a:spcBef>
+                  <a:spcAft>
+                    <a:spcPts val="0"/>
+                  </a:spcAft>
+                  <a:buClrTx/>
+                  <a:buSzTx/>
+                  <a:buFontTx/>
+                  <a:buNone/>
+                  <a:tabLst/>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="window" lastClr="FFFFFF"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="window" lastClr="FFFFFF"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t> |steps|</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                <a:lnSpc>
+                  <a:spcPct val="100000"/>
+                </a:lnSpc>
+                <a:spcBef>
+                  <a:spcPts val="0"/>
+                </a:spcBef>
+                <a:spcAft>
+                  <a:spcPts val="0"/>
+                </a:spcAft>
+                <a:buClrTx/>
+                <a:buSzTx/>
+                <a:buFontTx/>
+                <a:buNone/>
+                <a:tabLst/>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="window" lastClr="FFFFFF"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1942007936"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1942007936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:alpha val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                  <a:lnSpc>
+                    <a:spcPct val="100000"/>
+                  </a:lnSpc>
+                  <a:spcBef>
+                    <a:spcPts val="0"/>
+                  </a:spcBef>
+                  <a:spcAft>
+                    <a:spcPts val="0"/>
+                  </a:spcAft>
+                  <a:buClrTx/>
+                  <a:buSzTx/>
+                  <a:buFontTx/>
+                  <a:buNone/>
+                  <a:tabLst/>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="window" lastClr="FFFFFF"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="window" lastClr="FFFFFF"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>|configs|</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                <a:lnSpc>
+                  <a:spcPct val="100000"/>
+                </a:lnSpc>
+                <a:spcBef>
+                  <a:spcPts val="0"/>
+                </a:spcBef>
+                <a:spcAft>
+                  <a:spcPts val="0"/>
+                </a:spcAft>
+                <a:buClrTx/>
+                <a:buSzTx/>
+                <a:buFontTx/>
+                <a:buNone/>
+                <a:tabLst/>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="window" lastClr="FFFFFF"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1942278720"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="accent1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="accent1"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
@@ -3854,6 +5176,412 @@
                 <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="lt1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:alpha val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1975510720"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1975510720"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:alpha val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Time taken (s) </a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1974682752"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="accent1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="accent1"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>queue_wo_fork!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Time taken (s)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:alpha val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw dist="25400" dir="2700000" algn="tl" rotWithShape="0">
+                <a:schemeClr val="accent1"/>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="22225">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>queue_wo_fork!$A$2:$A$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>queue_wo_fork!$B$2:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5999999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.3000000000000002E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.7160000000000001E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C109-B642-8F21-2E1BD62E3881}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1974682752"/>
+        <c:axId val="1975510720"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1974682752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:alpha val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                  <a:lnSpc>
+                    <a:spcPct val="100000"/>
+                  </a:lnSpc>
+                  <a:spcBef>
+                    <a:spcPts val="0"/>
+                  </a:spcBef>
+                  <a:spcAft>
+                    <a:spcPts val="0"/>
+                  </a:spcAft>
+                  <a:buClrTx/>
+                  <a:buSzTx/>
+                  <a:buFontTx/>
+                  <a:buNone/>
+                  <a:tabLst/>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="window" lastClr="FFFFFF"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="window" lastClr="FFFFFF"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t> |steps|</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                <a:lnSpc>
+                  <a:spcPct val="100000"/>
+                </a:lnSpc>
+                <a:spcBef>
+                  <a:spcPts val="0"/>
+                </a:spcBef>
+                <a:spcAft>
+                  <a:spcPts val="0"/>
+                </a:spcAft>
+                <a:buClrTx/>
+                <a:buSzTx/>
+                <a:buFontTx/>
+                <a:buNone/>
+                <a:tabLst/>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="window" lastClr="FFFFFF"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -7461,7 +9189,167 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors17.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors18.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors19.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors20.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -12061,7 +13949,2147 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style17.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="247">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="0" kern="1200" spc="100" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <cs:styleClr val="auto"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltUpDiag">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltUpDiag">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+      <a:effectLst>
+        <a:outerShdw dist="25400" dir="2700000" algn="tl" rotWithShape="0">
+          <a:schemeClr val="phClr"/>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="22225">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="35000"/>
+          <a:lumOff val="65000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="79000">
+              <a:schemeClr val="phClr"/>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:alpha val="60000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="25400">
+          <a:schemeClr val="lt1"/>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+            <a:tint val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1500" b="1" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style18.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="247">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="0" kern="1200" spc="100" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <cs:styleClr val="auto"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltUpDiag">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltUpDiag">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+      <a:effectLst>
+        <a:outerShdw dist="25400" dir="2700000" algn="tl" rotWithShape="0">
+          <a:schemeClr val="phClr"/>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="22225">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="35000"/>
+          <a:lumOff val="65000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="79000">
+              <a:schemeClr val="phClr"/>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:alpha val="60000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="25400">
+          <a:schemeClr val="lt1"/>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+            <a:tint val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1500" b="1" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style19.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="247">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="0" kern="1200" spc="100" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <cs:styleClr val="auto"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltUpDiag">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltUpDiag">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+      <a:effectLst>
+        <a:outerShdw dist="25400" dir="2700000" algn="tl" rotWithShape="0">
+          <a:schemeClr val="phClr"/>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="22225">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="35000"/>
+          <a:lumOff val="65000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="79000">
+              <a:schemeClr val="phClr"/>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:alpha val="60000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="25400">
+          <a:schemeClr val="lt1"/>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+            <a:tint val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1500" b="1" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="247">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="0" kern="1200" spc="100" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <cs:styleClr val="auto"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltUpDiag">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltUpDiag">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+      <a:effectLst>
+        <a:outerShdw dist="25400" dir="2700000" algn="tl" rotWithShape="0">
+          <a:schemeClr val="phClr"/>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="22225">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="35000"/>
+          <a:lumOff val="65000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="79000">
+              <a:schemeClr val="phClr"/>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:alpha val="60000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="25400">
+          <a:schemeClr val="lt1"/>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+            <a:tint val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1500" b="1" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style20.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="247">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -16404,6 +20432,87 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>21166</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>10585</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>243417</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>10583</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{176F210F-02AF-E24C-875A-F8DBC17D8169}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>814917</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>189440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>814917</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>169333</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B336133E-863F-B14A-80B3-0DE9E2C7BC42}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -16987,6 +21096,87 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>21166</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>10585</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>243417</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>10583</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3854538C-A521-E94F-A951-572EBEFAFB91}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>814917</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>189440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>814917</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>169333</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B62E921-EA2A-4342-AB78-DDFF22A2CE71}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -17307,7 +21497,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C8" sqref="C8:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17401,7 +21591,7 @@
       <c r="B8">
         <v>0.32300400000000001</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="5" t="s">
         <v>1</v>
       </c>
     </row>
@@ -17412,7 +21602,7 @@
       <c r="B9">
         <v>0.70111800000000002</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="5" t="s">
         <v>1</v>
       </c>
     </row>
@@ -17423,7 +21613,7 @@
       <c r="B10">
         <v>1.383759</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="5" t="s">
         <v>1</v>
       </c>
     </row>
@@ -17434,7 +21624,7 @@
       <c r="B11">
         <v>2.1781890000000002</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="5" t="s">
         <v>1</v>
       </c>
     </row>
@@ -17445,13 +21635,178 @@
       <c r="B12">
         <v>3.381596</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="5" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2AD48C2-335E-2A4A-BB73-065EFB3FAC23}">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18.5" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1.5999999999999999E-5</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>4.3000000000000002E-5</v>
+      </c>
+      <c r="C4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>1.7160000000000001E-3</v>
+      </c>
+      <c r="C5">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>1.4859999999999999E-3</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>2.2780000000000001E-3</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>3.3240000000000001E-3</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>5.6340000000000001E-3</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>7.0270000000000003E-3</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>9.9389999999999999E-3</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>1.1586000000000001E-2</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{413E06AA-194E-BA4D-AE97-174D110D1F61}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -17460,7 +21815,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:A12"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17841,7 +22196,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17970,7 +22325,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18053,7 +22408,7 @@
       <c r="B7">
         <v>3.0379E-2</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="5" t="s">
         <v>1</v>
       </c>
     </row>
@@ -18064,7 +22419,7 @@
       <c r="B8">
         <v>6.0019000000000003E-2</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="5" t="s">
         <v>1</v>
       </c>
     </row>
@@ -18075,7 +22430,7 @@
       <c r="B9">
         <v>0.112465</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="5" t="s">
         <v>1</v>
       </c>
     </row>
@@ -18086,7 +22441,7 @@
       <c r="B10">
         <v>0.16463800000000001</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="5" t="s">
         <v>1</v>
       </c>
     </row>
@@ -18097,7 +22452,7 @@
       <c r="B11">
         <v>0.236156</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="5" t="s">
         <v>1</v>
       </c>
     </row>
@@ -18108,7 +22463,7 @@
       <c r="B12">
         <v>0.36367300000000002</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="5" t="s">
         <v>1</v>
       </c>
     </row>
@@ -18248,8 +22603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99A2615F-4FBC-8244-A8B0-B0706D1FDE93}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18371,13 +22726,127 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{413E06AA-194E-BA4D-AE97-174D110D1F61}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A61C4098-81E2-2C40-B07B-BBC948A0705C}">
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18.5" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2.5000000000000001E-5</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>5.8999999999999998E-5</v>
+      </c>
+      <c r="C4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>1.0449999999999999E-3</v>
+      </c>
+      <c r="C5">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>3.4667000000000003E-2</v>
+      </c>
+      <c r="C6">
+        <v>6784</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>1.5190999999999999</v>
+      </c>
+      <c r="C7">
+        <v>246560</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>141.505155</v>
+      </c>
+      <c r="C8" s="2">
+        <v>11852544</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C12" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>